<commit_message>
comments added and document finalized
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,30 +8,49 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swapn/Programming/Java/Adv-java-assignment3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D97C9AC-5C2E-C844-8245-32E3E98DB0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317B49FB-25BD-0545-A00A-D3454CDFCD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29700" yWindow="-2460" windowWidth="36020" windowHeight="19240" xr2:uid="{6FD445E1-EB57-A94A-A11A-CD5890AE6598}"/>
+    <workbookView xWindow="32720" yWindow="-2480" windowWidth="34480" windowHeight="19240" xr2:uid="{6FD445E1-EB57-A94A-A11A-CD5890AE6598}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$2:$C$6</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1266,15 +1285,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>373063</xdr:colOff>
+      <xdr:colOff>349251</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>174625</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>571226</xdr:colOff>
+      <xdr:colOff>547414</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>35650</xdr:rowOff>
+      <xdr:rowOff>3900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1297,7 +1316,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5016501" y="587375"/>
+          <a:off x="4992689" y="555625"/>
           <a:ext cx="8580163" cy="1924775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1610,7 +1629,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
done for Integer and character
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,50 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swapn/Programming/Java/Adv-java-assignment3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317B49FB-25BD-0545-A00A-D3454CDFCD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67816CEE-D6EA-3C4F-B2FB-6181D669575D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32720" yWindow="-2480" windowWidth="34480" windowHeight="19240" xr2:uid="{6FD445E1-EB57-A94A-A11A-CD5890AE6598}"/>
+    <workbookView xWindow="30160" yWindow="-2120" windowWidth="34480" windowHeight="19240" xr2:uid="{6FD445E1-EB57-A94A-A11A-CD5890AE6598}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Integer" sheetId="1" r:id="rId1"/>
+    <sheet name="Float" sheetId="2" r:id="rId2"/>
+    <sheet name="Character" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$2:$C$6</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$C$2:$C$6</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$C$2:$C$6</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$C$2:$C$6</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$6</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -73,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>Size</t>
   </si>
@@ -224,7 +189,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Integer!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -259,7 +224,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Integer!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -283,24 +248,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Integer!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.78025</c:v>
+                  <c:v>0.60445800000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24433299999999999</c:v>
+                  <c:v>2.5902500000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.10425</c:v>
+                  <c:v>2.3895420000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28783399999999998</c:v>
+                  <c:v>1.537541</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3597090000000001</c:v>
+                  <c:v>2.9736250000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -317,7 +282,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Integer!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -352,7 +317,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Integer!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -376,24 +341,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Integer!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15.369</c:v>
+                  <c:v>16.831666999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1063329999999998</c:v>
+                  <c:v>34.851958000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5996249999999996</c:v>
+                  <c:v>17.724457999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.432625</c:v>
+                  <c:v>8.3272499999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5854160000000004</c:v>
+                  <c:v>13.179874999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,7 +375,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Integer!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -445,7 +410,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Integer!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -469,24 +434,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:f>Integer!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>11.077500000000001</c:v>
+                  <c:v>6.4005000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0702500000000001</c:v>
+                  <c:v>17.645499999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.839791999999999</c:v>
+                  <c:v>11.990791</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4911670000000008</c:v>
+                  <c:v>11.30425</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.183292</c:v>
+                  <c:v>9.390625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,6 +460,1130 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A37B-1F43-8839-3A59F5F4F2FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1756386208"/>
+        <c:axId val="957902768"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1756386208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="957902768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="957902768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1756386208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> comparision of various Quick Sort implementation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Integer!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Integer!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Integer!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.60445800000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5902500000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3895420000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.537541</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9736250000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5046-3F48-B94C-DC6A7B33B669}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Integer!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parallel Quick Sort </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Integer!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Integer!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16.831666999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.851958000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.724457999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3272499999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.179874999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5046-3F48-B94C-DC6A7B33B669}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Integer!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thread Pooled Parallel Quick Sort </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Integer!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Integer!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.4005000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.645499999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.990791</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.30425</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.390625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5046-3F48-B94C-DC6A7B33B669}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1756386208"/>
+        <c:axId val="957902768"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1756386208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="957902768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="957902768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1756386208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> comparision of various Quick Sort implementation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Integer!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Integer!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Integer!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.60445800000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5902500000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3895420000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.537541</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9736250000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2530-C84F-A3FC-14A0754B5260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Integer!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parallel Quick Sort </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Integer!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Integer!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16.831666999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.851958000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.724457999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3272499999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.179874999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2530-C84F-A3FC-14A0754B5260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Integer!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thread Pooled Parallel Quick Sort </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Integer!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Integer!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.4005000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.645499999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.990791</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.30425</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.390625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2530-C84F-A3FC-14A0754B5260}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -741,7 +1830,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1285,22 +3460,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>349251</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>547414</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>3900</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>115543</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC66A5C-A90C-0672-9AF5-9F0AD748C67F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A957DD3-1C7B-17F4-FECC-A7B7DA3E092A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,14 +3491,100 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4992689" y="555625"/>
-          <a:ext cx="8580163" cy="1924775"/>
+          <a:off x="5024438" y="722312"/>
+          <a:ext cx="5640043" cy="2278063"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>5557</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>134938</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0E75055-1426-8A46-A6D7-AAB9E595D06C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>5557</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>134938</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{330FB771-2D84-4B47-B903-78A9110BAE90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1626,10 +3887,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2485F8-913E-2140-867E-CD04005D8FAB}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="11" max="11" width="1.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>0.60445800000000005</v>
+      </c>
+      <c r="C2">
+        <v>16.831666999999999</v>
+      </c>
+      <c r="D2">
+        <v>6.4005000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3">
+        <v>2.5902500000000002</v>
+      </c>
+      <c r="C3">
+        <v>34.851958000000003</v>
+      </c>
+      <c r="D3">
+        <v>17.645499999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>2.3895420000000001</v>
+      </c>
+      <c r="C4">
+        <v>17.724457999999998</v>
+      </c>
+      <c r="D4">
+        <v>11.990791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2500</v>
+      </c>
+      <c r="B5">
+        <v>1.537541</v>
+      </c>
+      <c r="C5">
+        <v>8.3272499999999994</v>
+      </c>
+      <c r="D5">
+        <v>11.30425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5000</v>
+      </c>
+      <c r="B6">
+        <v>2.9736250000000002</v>
+      </c>
+      <c r="C6">
+        <v>13.179874999999999</v>
+      </c>
+      <c r="D6">
+        <v>9.390625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1.61</v>
+      </c>
+      <c r="B7">
+        <v>13.94675</v>
+      </c>
+      <c r="C7">
+        <v>11.1845</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBE8EF4-D5D8-4D4A-A082-365631AB514D}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1638,7 +4017,6 @@
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1660,13 +4038,13 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>0.78025</v>
+        <v>0.60445800000000005</v>
       </c>
       <c r="C2">
-        <v>15.369</v>
+        <v>16.831666999999999</v>
       </c>
       <c r="D2">
-        <v>11.077500000000001</v>
+        <v>6.4005000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1674,13 +4052,13 @@
         <v>500</v>
       </c>
       <c r="B3">
-        <v>0.24433299999999999</v>
+        <v>2.5902500000000002</v>
       </c>
       <c r="C3">
-        <v>3.1063329999999998</v>
+        <v>34.851958000000003</v>
       </c>
       <c r="D3">
-        <v>3.0702500000000001</v>
+        <v>17.645499999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1688,13 +4066,13 @@
         <v>1000</v>
       </c>
       <c r="B4">
-        <v>3.10425</v>
+        <v>2.3895420000000001</v>
       </c>
       <c r="C4">
-        <v>9.5996249999999996</v>
+        <v>17.724457999999998</v>
       </c>
       <c r="D4">
-        <v>13.839791999999999</v>
+        <v>11.990791</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1702,13 +4080,13 @@
         <v>2500</v>
       </c>
       <c r="B5">
-        <v>0.28783399999999998</v>
+        <v>1.537541</v>
       </c>
       <c r="C5">
-        <v>15.432625</v>
+        <v>8.3272499999999994</v>
       </c>
       <c r="D5">
-        <v>8.4911670000000008</v>
+        <v>11.30425</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1716,13 +4094,141 @@
         <v>5000</v>
       </c>
       <c r="B6">
-        <v>1.3597090000000001</v>
+        <v>2.9736250000000002</v>
       </c>
       <c r="C6">
-        <v>4.5854160000000004</v>
+        <v>13.179874999999999</v>
       </c>
       <c r="D6">
-        <v>15.183292</v>
+        <v>9.390625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1.61</v>
+      </c>
+      <c r="B7">
+        <v>13.94675</v>
+      </c>
+      <c r="C7">
+        <v>11.1845</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0AF531-55D3-9E46-A332-2942F0854243}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>2.4834589999999999</v>
+      </c>
+      <c r="C2">
+        <v>2.4902920000000002</v>
+      </c>
+      <c r="D2">
+        <v>7.2995830000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3">
+        <v>0.54462500000000003</v>
+      </c>
+      <c r="C3">
+        <v>8.4205419999999993</v>
+      </c>
+      <c r="D3">
+        <v>2.1494580000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>4.0430000000000001</v>
+      </c>
+      <c r="C4">
+        <v>6.0788330000000004</v>
+      </c>
+      <c r="D4">
+        <v>15.447708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2500</v>
+      </c>
+      <c r="B5">
+        <v>6.7378340000000003</v>
+      </c>
+      <c r="C5">
+        <v>27.481000000000002</v>
+      </c>
+      <c r="D5">
+        <v>21.937833999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5000</v>
+      </c>
+      <c r="B6">
+        <v>2.687792</v>
+      </c>
+      <c r="C6">
+        <v>59.311250000000001</v>
+      </c>
+      <c r="D6">
+        <v>32.986584000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1.61</v>
+      </c>
+      <c r="B7">
+        <v>13.94675</v>
+      </c>
+      <c r="C7">
+        <v>11.1845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>